<commit_message>
Deletion of excess files and uploading image with path
Deleted files that were not used anymore and changed to direct image path instead of a particular name. There is still a bug because the image is in another folder.
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/plots_per_month/data_results.xlsx
+++ b/code/results/2021_monthly_results/plots_per_month/data_results.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
-  <si>
-    <t>Male Wildtype</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Male Null(-) </t>
   </si>
   <si>
     <t>Age</t>
@@ -25,34 +25,19 @@
     <t>mice #</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Female Wildtype</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Male Heterozygous</t>
-  </si>
-  <si>
-    <t>38</t>
+    <t xml:space="preserve">Female Null(-) </t>
+  </si>
+  <si>
+    <t>Male R403Q(+/-)</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Female Heterozygous</t>
+    <t>Female R403Q(+/-)</t>
   </si>
   <si>
     <t>6</t>
@@ -129,49 +114,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304809</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="May_histogram.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315200" y="0"/>
-          <a:ext cx="4572009" cy="4572009"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,15 +413,15 @@
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -510,51 +452,17 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -565,6 +473,5 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automatic addition of image based timeframe selected
Corrected bug were the graph figure  is saved based on the dates that are asked for.
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/plots_per_month/data_results.xlsx
+++ b/code/results/2021_monthly_results/plots_per_month/data_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t xml:space="preserve">Male Null(-) </t>
   </si>
@@ -25,13 +25,28 @@
     <t>mice #</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Female Null(-) </t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Male R403Q(+/-)</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>3</t>
@@ -114,6 +129,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>487690</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>182890</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="February-June.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="0"/>
+          <a:ext cx="4754890" cy="4754890"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,15 +471,15 @@
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -452,17 +510,45 @@
       </c>
     </row>
     <row r="3" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="D4" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -473,5 +559,6 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>